<commit_message>
Questions corrected, correctAnswer highlighted
</commit_message>
<xml_diff>
--- a/public/erste-hilfe-quiz-fragen-carsten-v1.xlsx
+++ b/public/erste-hilfe-quiz-fragen-carsten-v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://smartcondata-my.sharepoint.com/personal/carsten_hennig_smartcondata_de/Documents/Desktop/JUH/EH-Quiz-App/erste-hilfe-quiz-app/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="14_{B14C1AAD-72D6-4D3B-87A6-36DD801A6984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EB806F2-D18F-441E-9644-5100FD18F31A}"/>
+  <xr:revisionPtr revIDLastSave="164" documentId="14_{B14C1AAD-72D6-4D3B-87A6-36DD801A6984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45AE9E66-C65A-4E8F-B63A-136A2E6A0D72}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5BDE19DB-3098-4B74-95F7-D08234BDD55C}"/>
   </bookViews>
@@ -113,9 +113,6 @@
     <t>Hitzewallungen und starkes Schwitzen</t>
   </si>
   <si>
-    <t>Starke Schmerzen in der Brust, Engegefühl im Herzbereich, Übelkeit, Erbrechen, Atemnot und Schmerzen im Obernauch, fahles Gesicht</t>
-  </si>
-  <si>
     <t>Warum bringt man eine bewusstlose Person in die stabile Seitenlage?</t>
   </si>
   <si>
@@ -125,27 +122,18 @@
     <t>Damit es die Person bequemer hat</t>
   </si>
   <si>
-    <t>Damit Blut und Erbrochenes abfließen können und die bewusstlose Person nicht daran erstickt</t>
-  </si>
-  <si>
     <t>Damit die Umstehenden die Person besser sehen können</t>
   </si>
   <si>
     <t>Was sollte man als Ersthelfer:in bei einem Herzstillstand tun?</t>
   </si>
   <si>
-    <t>Notruf absetzen und weiteres abwarten</t>
-  </si>
-  <si>
     <t>Angehörige oder Zeugen trösten</t>
   </si>
   <si>
     <t>Abwechselnd 1x Mund-zu-Mund-Beatmung und 1x Herzdruckmassage im Wechsel</t>
   </si>
   <si>
-    <t>30x Herzdruckmassage, 2x Mund-zu-Mund-Beatmung im Wechsel</t>
-  </si>
-  <si>
     <t>Was ist die richtige Erste Hilfe bei einem Schock?</t>
   </si>
   <si>
@@ -317,9 +305,6 @@
     <t>Die Person zu zweit wegtragen</t>
   </si>
   <si>
-    <t>Unter den Achseln der Person durchgreifen, den Unterarm von oben fassen, die Person anheben und wegschleifen</t>
-  </si>
-  <si>
     <t>Was macht man bei Nasenbluten?</t>
   </si>
   <si>
@@ -332,9 +317,6 @@
     <t>Kalte Wadenwickel</t>
   </si>
   <si>
-    <t>Nasenlöcher mit vielen Taschntüchern zustopfen</t>
-  </si>
-  <si>
     <t>Eine bewusstlose Person atmtet regelmäßig / ausreichend. Wie wird sie gelagert?</t>
   </si>
   <si>
@@ -374,9 +356,6 @@
     <t>Einmalhandschuhe</t>
   </si>
   <si>
-    <t>Ein Erwachsener hat ein Stück Fleisch verschluckt und kann weder atmen noch sprechen. Was sollten Sie als Ersthelfender unverzüglich tun?</t>
-  </si>
-  <si>
     <t>Oberkörperhochlagerung</t>
   </si>
   <si>
@@ -414,6 +393,27 @@
   </si>
   <si>
     <t>Wie lautet die Nummer des Notrufs?</t>
+  </si>
+  <si>
+    <t>Starke Schmerzen in der Brust, Engegefühl im Herzbereich/Brustkorb, Übelkeit, Erbrechen, Atemnot und Schmerzen im Oberbauch, fahles Gesicht</t>
+  </si>
+  <si>
+    <t>Um die Atemwege frei zu machen und damit Blut und Erbrochenes abfließen können und die bewusstlose Person nicht daran erstickt</t>
+  </si>
+  <si>
+    <t>Notruf absetzen, Hilfe holen, Defi holen lassen, 30x Herzdruckmassage, 2x Mund-zu-Mund-Beatmung im Wechsel</t>
+  </si>
+  <si>
+    <t>Da kann man nichts machen</t>
+  </si>
+  <si>
+    <t>Unter den Achseln der Person durchgreifen, den Unterarm von oben fassen (Daumen oben lassen!), die Person anheben und wegschleifen</t>
+  </si>
+  <si>
+    <t>Nasenlöcher mit vielen Taschentüchern zustopfen</t>
+  </si>
+  <si>
+    <t>Eine Person hat ein Stück Fleisch verschluckt und kann weder atmen noch sprechen. Was sollten Sie als Ersthelfender unverzüglich tun?</t>
   </si>
 </sst>
 </file>
@@ -800,7 +800,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -834,7 +834,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B2">
         <v>110</v>
@@ -926,7 +926,7 @@
         <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>119</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -934,19 +934,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7" t="s">
         <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>30</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -954,19 +954,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
         <v>31</v>
       </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>34</v>
-      </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>121</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -974,19 +974,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
         <v>36</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" t="s">
-        <v>40</v>
       </c>
       <c r="F9">
         <v>3</v>
@@ -994,19 +994,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
         <v>41</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" t="s">
-        <v>45</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1014,19 +1014,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" t="s">
         <v>46</v>
-      </c>
-      <c r="B11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" t="s">
-        <v>50</v>
       </c>
       <c r="F11">
         <v>3</v>
@@ -1034,19 +1034,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E12" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F12">
         <v>2</v>
@@ -1054,19 +1054,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" t="s">
         <v>55</v>
-      </c>
-      <c r="B13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" t="s">
-        <v>59</v>
       </c>
       <c r="F13">
         <v>4</v>
@@ -1074,19 +1074,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="F14">
         <v>4</v>
@@ -1094,19 +1094,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" t="s">
         <v>64</v>
-      </c>
-      <c r="B15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" t="s">
-        <v>68</v>
       </c>
       <c r="F15">
         <v>3</v>
@@ -1114,19 +1114,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1134,19 +1134,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" t="s">
         <v>73</v>
-      </c>
-      <c r="B17" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" t="s">
-        <v>76</v>
-      </c>
-      <c r="E17" t="s">
-        <v>77</v>
       </c>
       <c r="F17">
         <v>3</v>
@@ -1154,19 +1154,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D18" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1174,19 +1174,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" t="s">
         <v>82</v>
-      </c>
-      <c r="B19" t="s">
-        <v>83</v>
-      </c>
-      <c r="C19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" t="s">
-        <v>86</v>
       </c>
       <c r="F19">
         <v>2</v>
@@ -1194,19 +1194,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E20" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="F20">
         <v>4</v>
@@ -1214,19 +1214,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D21" t="s">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="E21" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="F21">
         <v>3</v>
@@ -1234,19 +1234,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C22" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D22" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E22" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="F22">
         <v>2</v>
@@ -1254,19 +1254,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B23" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C23" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D23" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F23">
         <v>4</v>
@@ -1274,19 +1274,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B24" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D24" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E24" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="F24">
         <v>4</v>
@@ -1294,19 +1294,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B25" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C25" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D25" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E25" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F25">
         <v>3</v>
@@ -1314,19 +1314,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="B26" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C26" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D26" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E26" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="F26">
         <v>4</v>

</xml_diff>